<commit_message>
feat: add document for manage order usecase
</commit_message>
<xml_diff>
--- a/Unit Test/Search-TestPlan.xlsx
+++ b/Unit Test/Search-TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\TKXDPM.KHMT.20231-23\Unit Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University-HUST\20231\TKXDPM\TKXDPM.KHMT.20231-23\Unit Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2B8E74-8B27-4495-88E2-6C0ED36AD0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6920E1F7-DCF1-43A1-87D8-6E16BC07314C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="7" xr2:uid="{BA49DA37-6C72-4F0C-8F29-A460207C1BDB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="4" activeTab="7" xr2:uid="{BA49DA37-6C72-4F0C-8F29-A460207C1BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
   <si>
     <t>1. Introduction</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Cutomer is seending search text</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>CheckAvailableMedia</t>
   </si>
 </sst>
 </file>
@@ -834,6 +840,24 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -849,38 +873,68 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -894,54 +948,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1782,7 +1788,7 @@
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.1811023622047245" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -1800,9 +1806,9 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="39" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +1820,7 @@
       <c r="G1" s="39"/>
       <c r="H1" s="39"/>
     </row>
-    <row r="2" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1824,7 +1830,7 @@
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="39"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
@@ -1834,7 +1840,7 @@
       <c r="G3" s="39"/>
       <c r="H3" s="39"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="39"/>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -1844,7 +1850,7 @@
       <c r="G4" s="39"/>
       <c r="H4" s="39"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="39"/>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
@@ -1854,7 +1860,7 @@
       <c r="G5" s="39"/>
       <c r="H5" s="39"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
@@ -1864,7 +1870,7 @@
       <c r="G6" s="39"/>
       <c r="H6" s="39"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="39"/>
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
@@ -1874,7 +1880,7 @@
       <c r="G7" s="39"/>
       <c r="H7" s="39"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -1884,7 +1890,7 @@
       <c r="G8" s="39"/>
       <c r="H8" s="39"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
@@ -1894,7 +1900,7 @@
       <c r="G9" s="39"/>
       <c r="H9" s="39"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="39"/>
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
@@ -1904,7 +1910,7 @@
       <c r="G10" s="39"/>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="39"/>
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
@@ -1914,7 +1920,7 @@
       <c r="G11" s="39"/>
       <c r="H11" s="39"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="39"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -1924,7 +1930,7 @@
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
@@ -1934,7 +1940,7 @@
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="39"/>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -1944,7 +1950,7 @@
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="39"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -1954,7 +1960,7 @@
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="39"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
@@ -1964,7 +1970,7 @@
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
@@ -1992,14 +1998,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="4" spans="4:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:5" ht="17" x14ac:dyDescent="0.4">
       <c r="E4" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D6">
         <v>1</v>
       </c>
@@ -2007,7 +2013,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D7">
         <v>2</v>
       </c>
@@ -2015,7 +2021,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D8">
         <v>3</v>
       </c>
@@ -2023,7 +2029,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D9">
         <v>4</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D10">
         <v>5</v>
       </c>
@@ -2059,22 +2065,22 @@
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="88" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.77734375" style="14"/>
+    <col min="1" max="16384" width="8.81640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>80</v>
       </c>
@@ -2086,7 +2092,7 @@
       <c r="G3" s="40"/>
       <c r="H3" s="40"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
@@ -2096,7 +2102,7 @@
       <c r="G4" s="40"/>
       <c r="H4" s="40"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="40"/>
       <c r="B5" s="40"/>
       <c r="C5" s="40"/>
@@ -2106,7 +2112,7 @@
       <c r="G5" s="40"/>
       <c r="H5" s="40"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="40"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
@@ -2116,7 +2122,7 @@
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
@@ -2126,7 +2132,7 @@
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="40"/>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
@@ -2136,7 +2142,7 @@
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="40"/>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
@@ -2146,7 +2152,7 @@
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="40"/>
       <c r="B10" s="40"/>
       <c r="C10" s="40"/>
@@ -2156,7 +2162,7 @@
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="40"/>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
@@ -2166,12 +2172,12 @@
       <c r="G11" s="40"/>
       <c r="H11" s="40"/>
     </row>
-    <row r="13" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="41" t="s">
         <v>5</v>
       </c>
@@ -2183,7 +2189,7 @@
       <c r="G14" s="41"/>
       <c r="H14" s="41"/>
     </row>
-    <row r="15" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="41"/>
       <c r="B15" s="41"/>
       <c r="C15" s="41"/>
@@ -2193,7 +2199,7 @@
       <c r="G15" s="41"/>
       <c r="H15" s="41"/>
     </row>
-    <row r="16" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="41"/>
       <c r="B16" s="41"/>
       <c r="C16" s="41"/>
@@ -2203,7 +2209,7 @@
       <c r="G16" s="41"/>
       <c r="H16" s="41"/>
     </row>
-    <row r="17" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="41"/>
       <c r="B17" s="41"/>
       <c r="C17" s="41"/>
@@ -2213,7 +2219,7 @@
       <c r="G17" s="41"/>
       <c r="H17" s="41"/>
     </row>
-    <row r="18" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="41"/>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
@@ -2223,7 +2229,7 @@
       <c r="G18" s="41"/>
       <c r="H18" s="41"/>
     </row>
-    <row r="19" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="41"/>
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
@@ -2233,7 +2239,7 @@
       <c r="G19" s="41"/>
       <c r="H19" s="41"/>
     </row>
-    <row r="20" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="41"/>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
@@ -2243,7 +2249,7 @@
       <c r="G20" s="41"/>
       <c r="H20" s="41"/>
     </row>
-    <row r="21" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="41"/>
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
@@ -2253,7 +2259,7 @@
       <c r="G21" s="41"/>
       <c r="H21" s="41"/>
     </row>
-    <row r="22" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="41"/>
       <c r="B22" s="41"/>
       <c r="C22" s="41"/>
@@ -2263,7 +2269,7 @@
       <c r="G22" s="41"/>
       <c r="H22" s="41"/>
     </row>
-    <row r="23" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="41"/>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
@@ -2273,7 +2279,7 @@
       <c r="G23" s="41"/>
       <c r="H23" s="41"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="41"/>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
@@ -2283,7 +2289,7 @@
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2293,12 +2299,12 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="42" t="s">
         <v>7</v>
       </c>
@@ -2310,7 +2316,7 @@
       <c r="G27" s="42"/>
       <c r="H27" s="42"/>
     </row>
-    <row r="28" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="42"/>
       <c r="B28" s="42"/>
       <c r="C28" s="42"/>
@@ -2320,7 +2326,7 @@
       <c r="G28" s="42"/>
       <c r="H28" s="42"/>
     </row>
-    <row r="29" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="42"/>
       <c r="B29" s="42"/>
       <c r="C29" s="42"/>
@@ -2330,7 +2336,7 @@
       <c r="G29" s="42"/>
       <c r="H29" s="42"/>
     </row>
-    <row r="30" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="42"/>
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
@@ -2340,7 +2346,7 @@
       <c r="G30" s="42"/>
       <c r="H30" s="42"/>
     </row>
-    <row r="31" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="42"/>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
@@ -2350,7 +2356,7 @@
       <c r="G31" s="42"/>
       <c r="H31" s="42"/>
     </row>
-    <row r="32" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="42"/>
       <c r="B32" s="42"/>
       <c r="C32" s="42"/>
@@ -2360,7 +2366,7 @@
       <c r="G32" s="42"/>
       <c r="H32" s="42"/>
     </row>
-    <row r="33" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2370,7 +2376,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>8</v>
       </c>
@@ -2382,7 +2388,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="43" t="s">
         <v>67</v>
       </c>
@@ -2394,7 +2400,7 @@
       <c r="G35" s="43"/>
       <c r="H35" s="43"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="43"/>
       <c r="B36" s="43"/>
       <c r="C36" s="43"/>
@@ -2404,7 +2410,7 @@
       <c r="G36" s="43"/>
       <c r="H36" s="43"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="43"/>
       <c r="B37" s="43"/>
       <c r="C37" s="43"/>
@@ -2414,7 +2420,7 @@
       <c r="G37" s="43"/>
       <c r="H37" s="43"/>
     </row>
-    <row r="38" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="43"/>
       <c r="B38" s="43"/>
       <c r="C38" s="43"/>
@@ -2424,7 +2430,7 @@
       <c r="G38" s="43"/>
       <c r="H38" s="43"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="43"/>
       <c r="B39" s="43"/>
       <c r="C39" s="43"/>
@@ -2434,7 +2440,7 @@
       <c r="G39" s="43"/>
       <c r="H39" s="43"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="43"/>
       <c r="B40" s="43"/>
       <c r="C40" s="43"/>
@@ -2444,7 +2450,7 @@
       <c r="G40" s="43"/>
       <c r="H40" s="43"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="43"/>
       <c r="B41" s="43"/>
       <c r="C41" s="43"/>
@@ -2454,7 +2460,7 @@
       <c r="G41" s="43"/>
       <c r="H41" s="43"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="43"/>
       <c r="B42" s="43"/>
       <c r="C42" s="43"/>
@@ -2464,7 +2470,7 @@
       <c r="G42" s="43"/>
       <c r="H42" s="43"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="43"/>
       <c r="B43" s="43"/>
       <c r="C43" s="43"/>
@@ -2474,7 +2480,7 @@
       <c r="G43" s="43"/>
       <c r="H43" s="43"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="43"/>
       <c r="B44" s="43"/>
       <c r="C44" s="43"/>
@@ -2484,7 +2490,7 @@
       <c r="G44" s="43"/>
       <c r="H44" s="43"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="43"/>
       <c r="B45" s="43"/>
       <c r="C45" s="43"/>
@@ -2494,7 +2500,7 @@
       <c r="G45" s="43"/>
       <c r="H45" s="43"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="43"/>
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
@@ -2504,7 +2510,7 @@
       <c r="G46" s="43"/>
       <c r="H46" s="43"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="43"/>
       <c r="B47" s="43"/>
       <c r="C47" s="43"/>
@@ -2514,7 +2520,7 @@
       <c r="G47" s="43"/>
       <c r="H47" s="43"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="43"/>
       <c r="B48" s="43"/>
       <c r="C48" s="43"/>
@@ -2524,7 +2530,7 @@
       <c r="G48" s="43"/>
       <c r="H48" s="43"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="43"/>
       <c r="B49" s="43"/>
       <c r="C49" s="43"/>
@@ -2556,22 +2562,22 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.77734375" style="5"/>
+    <col min="1" max="16384" width="8.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="44" t="s">
         <v>10</v>
       </c>
@@ -2583,7 +2589,7 @@
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="44"/>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -2593,7 +2599,7 @@
       <c r="G4" s="44"/>
       <c r="H4" s="44"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -2603,7 +2609,7 @@
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -2613,7 +2619,7 @@
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="44"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
@@ -2623,7 +2629,7 @@
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -2633,7 +2639,7 @@
       <c r="G8" s="44"/>
       <c r="H8" s="44"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
@@ -2643,7 +2649,7 @@
       <c r="G9" s="44"/>
       <c r="H9" s="44"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="44"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -2653,7 +2659,7 @@
       <c r="G10" s="44"/>
       <c r="H10" s="44"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -2663,17 +2669,17 @@
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
     </row>
-    <row r="13" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="45" t="s">
         <v>12</v>
       </c>
@@ -2685,7 +2691,7 @@
       <c r="G15" s="45"/>
       <c r="H15" s="45"/>
     </row>
-    <row r="16" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="45"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
@@ -2695,7 +2701,7 @@
       <c r="G16" s="45"/>
       <c r="H16" s="45"/>
     </row>
-    <row r="17" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="45"/>
       <c r="B17" s="45"/>
       <c r="C17" s="45"/>
@@ -2705,7 +2711,7 @@
       <c r="G17" s="45"/>
       <c r="H17" s="45"/>
     </row>
-    <row r="18" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="45"/>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
@@ -2715,7 +2721,7 @@
       <c r="G18" s="45"/>
       <c r="H18" s="45"/>
     </row>
-    <row r="19" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="45"/>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
@@ -2725,7 +2731,7 @@
       <c r="G19" s="45"/>
       <c r="H19" s="45"/>
     </row>
-    <row r="20" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -2735,7 +2741,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>14</v>
       </c>
@@ -2747,7 +2753,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="46" t="s">
         <v>15</v>
       </c>
@@ -2759,7 +2765,7 @@
       <c r="G22" s="46"/>
       <c r="H22" s="46"/>
     </row>
-    <row r="23" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="46"/>
       <c r="B23" s="46"/>
       <c r="C23" s="46"/>
@@ -2769,7 +2775,7 @@
       <c r="G23" s="46"/>
       <c r="H23" s="46"/>
     </row>
-    <row r="24" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="46"/>
       <c r="B24" s="46"/>
       <c r="C24" s="46"/>
@@ -2779,7 +2785,7 @@
       <c r="G24" s="46"/>
       <c r="H24" s="46"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="46"/>
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
@@ -2789,7 +2795,7 @@
       <c r="G25" s="46"/>
       <c r="H25" s="46"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="46"/>
       <c r="B26" s="46"/>
       <c r="C26" s="46"/>
@@ -2799,7 +2805,7 @@
       <c r="G26" s="46"/>
       <c r="H26" s="46"/>
     </row>
-    <row r="27" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="46"/>
       <c r="B27" s="46"/>
       <c r="C27" s="46"/>
@@ -2809,7 +2815,7 @@
       <c r="G27" s="46"/>
       <c r="H27" s="46"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="46"/>
       <c r="B28" s="46"/>
       <c r="C28" s="46"/>
@@ -2819,7 +2825,7 @@
       <c r="G28" s="46"/>
       <c r="H28" s="46"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="46"/>
       <c r="B29" s="46"/>
       <c r="C29" s="46"/>
@@ -2829,7 +2835,7 @@
       <c r="G29" s="46"/>
       <c r="H29" s="46"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="46"/>
       <c r="B30" s="46"/>
       <c r="C30" s="46"/>
@@ -2839,7 +2845,7 @@
       <c r="G30" s="46"/>
       <c r="H30" s="46"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="46"/>
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
@@ -2849,7 +2855,7 @@
       <c r="G31" s="46"/>
       <c r="H31" s="46"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="46"/>
       <c r="B32" s="46"/>
       <c r="C32" s="46"/>
@@ -2859,7 +2865,7 @@
       <c r="G32" s="46"/>
       <c r="H32" s="46"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="46"/>
       <c r="B33" s="46"/>
       <c r="C33" s="46"/>
@@ -2869,7 +2875,7 @@
       <c r="G33" s="46"/>
       <c r="H33" s="46"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="46"/>
       <c r="B34" s="46"/>
       <c r="C34" s="46"/>
@@ -2879,7 +2885,7 @@
       <c r="G34" s="46"/>
       <c r="H34" s="46"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>16</v>
       </c>
@@ -2891,7 +2897,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="46" t="s">
         <v>17</v>
       </c>
@@ -2903,7 +2909,7 @@
       <c r="G36" s="46"/>
       <c r="H36" s="46"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="46"/>
       <c r="B37" s="46"/>
       <c r="C37" s="46"/>
@@ -2913,7 +2919,7 @@
       <c r="G37" s="46"/>
       <c r="H37" s="46"/>
     </row>
-    <row r="38" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="46"/>
       <c r="B38" s="46"/>
       <c r="C38" s="46"/>
@@ -2923,7 +2929,7 @@
       <c r="G38" s="46"/>
       <c r="H38" s="46"/>
     </row>
-    <row r="39" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="46"/>
       <c r="B39" s="46"/>
       <c r="C39" s="46"/>
@@ -2933,7 +2939,7 @@
       <c r="G39" s="46"/>
       <c r="H39" s="46"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2943,7 +2949,7 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2953,7 +2959,7 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2963,7 +2969,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2973,7 +2979,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2983,7 +2989,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2993,7 +2999,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -3003,7 +3009,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3013,7 +3019,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -3023,7 +3029,7 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -3033,7 +3039,7 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -3043,7 +3049,7 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -3074,14 +3080,14 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>19</v>
       </c>
@@ -3093,7 +3099,7 @@
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="47"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -3103,7 +3109,7 @@
       <c r="G3" s="47"/>
       <c r="H3" s="47"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="47"/>
       <c r="B4" s="47"/>
       <c r="C4" s="47"/>
@@ -3113,7 +3119,7 @@
       <c r="G4" s="47"/>
       <c r="H4" s="47"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="47"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
@@ -3123,7 +3129,7 @@
       <c r="G5" s="47"/>
       <c r="H5" s="47"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="47"/>
       <c r="B6" s="47"/>
       <c r="C6" s="47"/>
@@ -3133,7 +3139,7 @@
       <c r="G6" s="47"/>
       <c r="H6" s="47"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="47"/>
       <c r="B7" s="47"/>
       <c r="C7" s="47"/>
@@ -3143,7 +3149,7 @@
       <c r="G7" s="47"/>
       <c r="H7" s="47"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="47"/>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
@@ -3153,7 +3159,7 @@
       <c r="G8" s="47"/>
       <c r="H8" s="47"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="47"/>
       <c r="B9" s="47"/>
       <c r="C9" s="47"/>
@@ -3163,7 +3169,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="47"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="47"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
@@ -3173,7 +3179,7 @@
       <c r="G10" s="47"/>
       <c r="H10" s="47"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="47"/>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
@@ -3183,7 +3189,7 @@
       <c r="G11" s="47"/>
       <c r="H11" s="47"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="47"/>
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
@@ -3193,7 +3199,7 @@
       <c r="G12" s="47"/>
       <c r="H12" s="47"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="47"/>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
@@ -3203,7 +3209,7 @@
       <c r="G13" s="47"/>
       <c r="H13" s="47"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="47"/>
       <c r="B14" s="47"/>
       <c r="C14" s="47"/>
@@ -3213,7 +3219,7 @@
       <c r="G14" s="47"/>
       <c r="H14" s="47"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="47"/>
       <c r="B15" s="47"/>
       <c r="C15" s="47"/>
@@ -3223,7 +3229,7 @@
       <c r="G15" s="47"/>
       <c r="H15" s="47"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="47"/>
       <c r="B16" s="47"/>
       <c r="C16" s="47"/>
@@ -3233,7 +3239,7 @@
       <c r="G16" s="47"/>
       <c r="H16" s="47"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="47"/>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -3243,7 +3249,7 @@
       <c r="G17" s="47"/>
       <c r="H17" s="47"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="47"/>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
@@ -3253,7 +3259,7 @@
       <c r="G18" s="47"/>
       <c r="H18" s="47"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="47"/>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
@@ -3263,7 +3269,7 @@
       <c r="G19" s="47"/>
       <c r="H19" s="47"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="47"/>
       <c r="B20" s="47"/>
       <c r="C20" s="47"/>
@@ -3273,7 +3279,7 @@
       <c r="G20" s="47"/>
       <c r="H20" s="47"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="47"/>
       <c r="B21" s="47"/>
       <c r="C21" s="47"/>
@@ -3283,7 +3289,7 @@
       <c r="G21" s="47"/>
       <c r="H21" s="47"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="47"/>
       <c r="B22" s="47"/>
       <c r="C22" s="47"/>
@@ -3306,41 +3312,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8917CA0A-EA61-4F09-84F9-F925FF2C64CE}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:I29"/>
+    <sheetView view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.21875" customWidth="1"/>
-    <col min="2" max="2" width="37.21875" customWidth="1"/>
-    <col min="4" max="9" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" customWidth="1"/>
+    <col min="4" max="9" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>77</v>
       </c>
       <c r="B2" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
         <v>68</v>
       </c>
       <c r="B3" s="11"/>
     </row>
-    <row r="4" spans="1:9" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56" t="s">
+    <row r="4" spans="1:9" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="58"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="35" t="s">
         <v>24</v>
       </c>
@@ -3360,7 +3366,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="18" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
         <v>29</v>
       </c>
@@ -3376,7 +3382,7 @@
       </c>
       <c r="E5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="17">
         <f t="shared" si="0"/>
@@ -3395,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>36</v>
       </c>
@@ -3417,18 +3423,26 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="17">
+        <v>1</v>
+      </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="E7" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3439,7 +3453,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -3450,7 +3464,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -3461,7 +3475,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -3472,54 +3486,54 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="54"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="53" t="s">
+      <c r="D15" s="52"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="55"/>
-    </row>
-    <row r="16" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="53"/>
+    </row>
+    <row r="16" spans="1:9" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51" t="s">
+      <c r="D16" s="55"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="52"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G16" s="58"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
@@ -3528,22 +3542,22 @@
       <c r="F19" s="23"/>
       <c r="G19" s="23"/>
     </row>
-    <row r="20" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.4">
       <c r="A20" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="56" t="s">
+    <row r="22" spans="1:9" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="58"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="35" t="s">
         <v>71</v>
       </c>
@@ -3563,7 +3577,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="36" t="s">
         <v>29</v>
       </c>
@@ -3598,13 +3612,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17">
-        <f t="shared" ref="C24:C29" si="2">COUNTIF(D24:R24,"=x")</f>
+        <f t="shared" ref="C24" si="2">COUNTIF(D24:R24,"=x")</f>
         <v>1</v>
       </c>
       <c r="D24" s="19" t="s">
@@ -3616,7 +3630,7 @@
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -3627,7 +3641,7 @@
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -3638,7 +3652,7 @@
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -3649,7 +3663,7 @@
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -3660,7 +3674,7 @@
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -3671,51 +3685,51 @@
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
         <v>65</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="53" t="s">
+      <c r="C33" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="54"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="53" t="s">
+      <c r="D33" s="52"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="55"/>
-    </row>
-    <row r="34" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="53"/>
+    </row>
+    <row r="34" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
         <v>78</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="48" t="s">
+      <c r="C34" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="49"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="51" t="s">
+      <c r="D34" s="55"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="G34" s="52"/>
-    </row>
-    <row r="35" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="58"/>
+    </row>
+    <row r="35" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="22"/>
@@ -3726,16 +3740,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="1.1811023622047243" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -3747,65 +3761,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF123E7-2EB5-48C5-B5DD-E8CB50F3BF35}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24:J24"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A42" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:J50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="2.77734375" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.6328125" customWidth="1"/>
+    <col min="2" max="2" width="2.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+    <row r="3" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="79"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="81" t="s">
+      <c r="E3" s="64"/>
+      <c r="F3" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="81"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="79"/>
+      <c r="B4" s="64"/>
       <c r="C4" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="79"/>
-      <c r="F4" s="80" t="s">
+      <c r="E4" s="64"/>
+      <c r="F4" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="80"/>
+      <c r="G4" s="65"/>
       <c r="H4" s="28" t="s">
         <v>41</v>
       </c>
@@ -3814,7 +3828,7 @@
       </c>
       <c r="J4" s="29"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="27"/>
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
@@ -3826,11 +3840,11 @@
       <c r="I5" s="27"/>
       <c r="J5" s="27"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="72" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="73"/>
+      <c r="B6" s="76"/>
       <c r="C6" s="26" t="s">
         <v>59</v>
       </c>
@@ -3842,7 +3856,7 @@
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="30"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
@@ -3854,22 +3868,22 @@
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
     </row>
-    <row r="8" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="74" t="s">
+    <row r="8" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="73"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="73"/>
-      <c r="F8" s="75" t="s">
+      <c r="E8" s="76"/>
+      <c r="F8" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="76"/>
+      <c r="G8" s="79"/>
       <c r="H8" s="28" t="s">
         <v>46</v>
       </c>
@@ -3877,7 +3891,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20" t="s">
@@ -3888,19 +3902,19 @@
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
     </row>
-    <row r="10" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-    </row>
-    <row r="11" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+    </row>
+    <row r="11" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32">
         <v>1</v>
       </c>
@@ -3912,7 +3926,7 @@
       <c r="E11" s="59"/>
       <c r="F11" s="59"/>
     </row>
-    <row r="12" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="32">
         <v>2</v>
       </c>
@@ -3924,7 +3938,7 @@
       <c r="E12" s="59"/>
       <c r="F12" s="59"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
@@ -3936,25 +3950,25 @@
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71" t="s">
+      <c r="C14" s="68"/>
+      <c r="D14" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="32">
         <v>1</v>
       </c>
@@ -3962,31 +3976,31 @@
         <v>99</v>
       </c>
       <c r="C15" s="59"/>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="32">
         <v>2</v>
       </c>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="84"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="74"/>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="32">
         <v>3</v>
       </c>
@@ -4000,23 +4014,23 @@
       <c r="I17" s="27"/>
       <c r="J17" s="27"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="34"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
       <c r="G18" s="26"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="63" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="63"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="26" t="s">
         <v>51</v>
       </c>
@@ -4028,51 +4042,51 @@
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C20" s="34"/>
     </row>
-    <row r="21" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="61" t="s">
+    <row r="21" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="66" t="s">
+      <c r="C21" s="80"/>
+      <c r="D21" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="67"/>
-      <c r="F21" s="69" t="s">
+      <c r="E21" s="83"/>
+      <c r="F21" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="69"/>
-      <c r="H21" s="61" t="s">
+      <c r="G21" s="62"/>
+      <c r="H21" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-    </row>
-    <row r="23" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="80"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+    </row>
+    <row r="23" spans="1:10" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="32">
         <v>1</v>
       </c>
       <c r="B23" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="60"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="59" t="s">
         <v>102</v>
       </c>
@@ -4087,10 +4101,10 @@
       <c r="I23" s="59"/>
       <c r="J23" s="59"/>
     </row>
-    <row r="24" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="32"/>
       <c r="B24" s="59"/>
-      <c r="C24" s="60"/>
+      <c r="C24" s="61"/>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
       <c r="F24" s="59"/>
@@ -4099,10 +4113,10 @@
       <c r="I24" s="59"/>
       <c r="J24" s="59"/>
     </row>
-    <row r="25" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="32"/>
       <c r="B25" s="59"/>
-      <c r="C25" s="60"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
       <c r="F25" s="59"/>
@@ -4113,6 +4127,34 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:E22"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="H25:J25"/>
@@ -4124,36 +4166,8 @@
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D23:E23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="D21:E22"/>
   </mergeCells>
   <pageMargins left="1.1811023622047245" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4161,18 +4175,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4393,14 +4407,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6913AF88-A569-4E93-8BD1-0040FA9C021A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8655864D-7A2A-4402-AA52-01C6DA779FC3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -4413,6 +4419,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6913AF88-A569-4E93-8BD1-0040FA9C021A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>